<commit_message>
more work on website
</commit_message>
<xml_diff>
--- a/backend/test.xlsx
+++ b/backend/test.xlsx
@@ -1998,7 +1998,7 @@
       <c r="D16" s="7" t="n"/>
       <c r="E16" s="15" t="inlineStr">
         <is>
-          <t>San Diego, CA 92104</t>
+          <t>San Diego ,CA 92104</t>
         </is>
       </c>
       <c r="F16" s="7" t="n"/>
@@ -2066,7 +2066,7 @@
       <c r="D20" s="21" t="n"/>
       <c r="E20" s="22" t="inlineStr">
         <is>
-          <t>REPLACE</t>
+          <t>49204808</t>
         </is>
       </c>
       <c r="F20" s="23" t="n"/>
@@ -2084,11 +2084,7 @@
       </c>
       <c r="C21" s="9" t="n"/>
       <c r="D21" s="7" t="n"/>
-      <c r="E21" s="24" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
+      <c r="E21" s="24" t="inlineStr"/>
       <c r="F21" s="7" t="n"/>
       <c r="G21" s="7" t="n"/>
       <c r="H21" s="13" t="n"/>
@@ -2126,7 +2122,7 @@
       <c r="D23" s="7" t="n"/>
       <c r="E23" s="25" t="inlineStr">
         <is>
-          <t>REPLACE</t>
+          <t>8/19/2024</t>
         </is>
       </c>
       <c r="F23" s="7" t="n"/>
@@ -2184,154 +2180,116 @@
       <c r="J25" s="2" t="n"/>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="63">
-      <c r="A26" s="10" t="inlineStr">
+      <c r="A26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" s="34" t="inlineStr">
+        <is>
+          <t>Cases</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="inlineStr"/>
+      <c r="D26" s="10" t="inlineStr">
         <is>
           <t>REPLACE</t>
         </is>
       </c>
-      <c r="B26" s="34" t="inlineStr">
-        <is>
-          <t>Cases</t>
-        </is>
-      </c>
-      <c r="C26" s="10" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
-      <c r="D26" s="10" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
       <c r="E26" s="68" t="n"/>
-      <c r="F26" s="10" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
-      <c r="G26" s="15" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
+      <c r="F26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="15" t="n">
+        <v>0</v>
       </c>
       <c r="H26" s="13" t="n"/>
       <c r="I26" s="13" t="n"/>
       <c r="J26" s="2" t="n"/>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="63">
-      <c r="A27" s="36" t="inlineStr">
+      <c r="A27" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="B27" s="37" t="inlineStr">
+        <is>
+          <t>Cases</t>
+        </is>
+      </c>
+      <c r="C27" s="36" t="inlineStr"/>
+      <c r="D27" s="36" t="inlineStr">
         <is>
           <t>REPLACE</t>
         </is>
       </c>
-      <c r="B27" s="37" t="inlineStr">
-        <is>
-          <t>Cases</t>
-        </is>
-      </c>
-      <c r="C27" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
-      <c r="D27" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
       <c r="E27" s="69" t="n"/>
-      <c r="F27" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
-      <c r="G27" s="10" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
+      <c r="F27" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="H27" s="13" t="n"/>
       <c r="I27" s="13" t="n"/>
       <c r="J27" s="2" t="n"/>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="63">
-      <c r="A28" s="36" t="inlineStr">
+      <c r="A28" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="B28" s="37" t="inlineStr">
+        <is>
+          <t>Cases</t>
+        </is>
+      </c>
+      <c r="C28" s="36" t="inlineStr"/>
+      <c r="D28" s="36" t="inlineStr">
         <is>
           <t>REPLACE</t>
         </is>
       </c>
-      <c r="B28" s="37" t="inlineStr">
-        <is>
-          <t>Cases</t>
-        </is>
-      </c>
-      <c r="C28" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
-      <c r="D28" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
       <c r="E28" s="69" t="n"/>
-      <c r="F28" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
-      <c r="G28" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
+      <c r="F28" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="36" t="n">
+        <v>0</v>
       </c>
       <c r="H28" s="13" t="n"/>
       <c r="I28" s="13" t="n"/>
       <c r="J28" s="2" t="n"/>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="63">
-      <c r="A29" s="36" t="inlineStr">
+      <c r="A29" s="36" t="n">
+        <v>150</v>
+      </c>
+      <c r="B29" s="37" t="inlineStr">
+        <is>
+          <t>Cases</t>
+        </is>
+      </c>
+      <c r="C29" s="36" t="inlineStr">
+        <is>
+          <t>10068</t>
+        </is>
+      </c>
+      <c r="D29" s="36" t="inlineStr">
         <is>
           <t>REPLACE</t>
         </is>
       </c>
-      <c r="B29" s="37" t="inlineStr">
-        <is>
-          <t>Cases</t>
-        </is>
-      </c>
-      <c r="C29" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
-      <c r="D29" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
       <c r="E29" s="69" t="n"/>
-      <c r="F29" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
-      </c>
-      <c r="G29" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
+      <c r="F29" s="36" t="n">
+        <v>450</v>
+      </c>
+      <c r="G29" s="36" t="n">
+        <v>67500</v>
       </c>
       <c r="H29" s="13" t="n"/>
       <c r="I29" s="13" t="n"/>
       <c r="J29" s="2" t="n"/>
     </row>
     <row r="30" ht="16.5" customHeight="1" s="63">
-      <c r="A30" s="36" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
+      <c r="A30" s="36" t="n">
+        <v>150</v>
       </c>
       <c r="B30" s="37" t="inlineStr">
         <is>
@@ -2346,10 +2304,8 @@
         </is>
       </c>
       <c r="F30" s="40" t="n"/>
-      <c r="G30" s="41" t="inlineStr">
-        <is>
-          <t>REPLACE</t>
-        </is>
+      <c r="G30" s="41" t="n">
+        <v>66150</v>
       </c>
       <c r="H30" s="13" t="n"/>
       <c r="I30" s="13" t="n"/>

</xml_diff>

<commit_message>
allowed exporting of excel file
</commit_message>
<xml_diff>
--- a/backend/test.xlsx
+++ b/backend/test.xlsx
@@ -1932,7 +1932,7 @@
       <c r="D14" s="7" t="n"/>
       <c r="E14" s="15" t="inlineStr">
         <is>
-          <t>UNFI - Dublin, CA</t>
+          <t>UNFI – Dublin, CA Appt:</t>
         </is>
       </c>
       <c r="F14" s="66" t="n"/>
@@ -1948,7 +1948,7 @@
       <c r="D15" s="7" t="n"/>
       <c r="E15" s="15" t="inlineStr">
         <is>
-          <t>4000 Inspiration Drive</t>
+          <t>dubappts@unfi.com</t>
         </is>
       </c>
       <c r="F15" s="66" t="n"/>
@@ -1964,7 +1964,7 @@
       <c r="D16" s="7" t="n"/>
       <c r="E16" s="15" t="inlineStr">
         <is>
-          <t>Dublin, CA 94568</t>
+          <t>4000 Inspiration Drive</t>
         </is>
       </c>
       <c r="F16" s="7" t="n"/>
@@ -1980,7 +1980,7 @@
       <c r="D17" s="7" t="n"/>
       <c r="E17" s="10" t="inlineStr">
         <is>
-          <t>REPLACE</t>
+          <t>Dublin, CA 94568</t>
         </is>
       </c>
       <c r="F17" s="7" t="n"/>
@@ -2050,11 +2050,7 @@
       </c>
       <c r="C21" s="9" t="n"/>
       <c r="D21" s="7" t="n"/>
-      <c r="E21" s="15" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="E21" s="15" t="inlineStr"/>
       <c r="F21" s="7" t="n"/>
       <c r="G21" s="7" t="n"/>
       <c r="H21" s="13" t="n"/>
@@ -2162,7 +2158,7 @@
       </c>
       <c r="C26" s="10" t="inlineStr">
         <is>
-          <t>02420</t>
+          <t>10827</t>
         </is>
       </c>
       <c r="D26" s="22" t="inlineStr">
@@ -2198,7 +2194,7 @@
       </c>
       <c r="C27" s="32" t="inlineStr">
         <is>
-          <t>02421</t>
+          <t>10829</t>
         </is>
       </c>
       <c r="D27" s="22" t="inlineStr">
@@ -2234,7 +2230,7 @@
       </c>
       <c r="C28" s="32" t="inlineStr">
         <is>
-          <t>100262</t>
+          <t>82058</t>
         </is>
       </c>
       <c r="D28" s="22" t="inlineStr">
@@ -2270,7 +2266,7 @@
       </c>
       <c r="C29" s="35" t="inlineStr">
         <is>
-          <t>10068</t>
+          <t>11311</t>
         </is>
       </c>
       <c r="D29" s="36" t="inlineStr">

</xml_diff>

<commit_message>
initiated firebase, added counting for internal tracking numbers
</commit_message>
<xml_diff>
--- a/backend/test.xlsx
+++ b/backend/test.xlsx
@@ -1932,7 +1932,7 @@
       <c r="D14" s="7" t="n"/>
       <c r="E14" s="15" t="inlineStr">
         <is>
-          <t>UNFI – Dublin, CA Appt:</t>
+          <t>UNFI – Dublin, CA</t>
         </is>
       </c>
       <c r="F14" s="66" t="n"/>
@@ -1948,7 +1948,7 @@
       <c r="D15" s="7" t="n"/>
       <c r="E15" s="15" t="inlineStr">
         <is>
-          <t>dubappts@unfi.com</t>
+          <t>4000 Inspiration Drive</t>
         </is>
       </c>
       <c r="F15" s="66" t="n"/>
@@ -1964,7 +1964,7 @@
       <c r="D16" s="7" t="n"/>
       <c r="E16" s="15" t="inlineStr">
         <is>
-          <t>4000 Inspiration Drive</t>
+          <t>Dublin, CA 94568</t>
         </is>
       </c>
       <c r="F16" s="7" t="n"/>
@@ -1980,7 +1980,7 @@
       <c r="D17" s="7" t="n"/>
       <c r="E17" s="10" t="inlineStr">
         <is>
-          <t>Dublin, CA 94568</t>
+          <t>REPLACE</t>
         </is>
       </c>
       <c r="F17" s="7" t="n"/>
@@ -2050,7 +2050,11 @@
       </c>
       <c r="C21" s="9" t="n"/>
       <c r="D21" s="7" t="n"/>
-      <c r="E21" s="15" t="inlineStr"/>
+      <c r="E21" s="15" t="inlineStr">
+        <is>
+          <t>08/01/24</t>
+        </is>
+      </c>
       <c r="F21" s="7" t="n"/>
       <c r="G21" s="7" t="n"/>
       <c r="H21" s="13" t="n"/>
@@ -2158,7 +2162,7 @@
       </c>
       <c r="C26" s="10" t="inlineStr">
         <is>
-          <t>10827</t>
+          <t>02420</t>
         </is>
       </c>
       <c r="D26" s="22" t="inlineStr">
@@ -2194,7 +2198,7 @@
       </c>
       <c r="C27" s="32" t="inlineStr">
         <is>
-          <t>10829</t>
+          <t>02421</t>
         </is>
       </c>
       <c r="D27" s="22" t="inlineStr">
@@ -2230,7 +2234,7 @@
       </c>
       <c r="C28" s="32" t="inlineStr">
         <is>
-          <t>82058</t>
+          <t>100262</t>
         </is>
       </c>
       <c r="D28" s="22" t="inlineStr">
@@ -2266,7 +2270,7 @@
       </c>
       <c r="C29" s="35" t="inlineStr">
         <is>
-          <t>11311</t>
+          <t>10068</t>
         </is>
       </c>
       <c r="D29" s="36" t="inlineStr">

</xml_diff>